<commit_message>
Add support for more than one HEADING variable
Close #12
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXSTA_small.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXSTA_small.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/672a29ec829a16e8/Dokumenter/GitHub/ProjCore/px/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C72DD2B6-B372-45B2-8244-0BD49BB7926D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{970C7768-B323-4910-9195-51823FB5551C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB298E7-0EB2-46CC-B479-454346DF6605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18900" yWindow="12450" windowWidth="17520" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -346,9 +346,6 @@
     <t>s1</t>
   </si>
   <si>
-    <t>s2</t>
-  </si>
-  <si>
     <t>www.stat.gl/bed202201/m1</t>
   </si>
   <si>
@@ -446,6 +443,9 @@
   </si>
   <si>
     <t>ANSI</t>
+  </si>
+  <si>
+    <t>h2</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Link 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -521,7 +521,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -843,11 +843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="5" width="30" customWidth="1"/>
@@ -966,13 +966,13 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J3" t="s">
         <v>83</v>
@@ -984,18 +984,18 @@
         <v>84</v>
       </c>
       <c r="M3" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" t="s">
         <v>137</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>138</v>
-      </c>
-      <c r="O3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>73</v>
@@ -1094,7 +1094,7 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -1122,7 +1122,7 @@
         <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1130,7 +1130,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
         <v>99</v>
@@ -1150,7 +1150,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -1170,7 +1170,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -1190,7 +1190,7 @@
         <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>99</v>
@@ -1210,7 +1210,7 @@
         <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>100</v>
@@ -1230,7 +1230,7 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>101</v>
@@ -1254,14 +1254,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.59765625" customWidth="1"/>
-    <col min="2" max="2" width="42.73046875" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1274,15 +1274,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="4">
         <v>2000</v>
@@ -1290,26 +1290,26 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1338,26 +1338,26 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1">
@@ -1365,7 +1365,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1">
@@ -1373,7 +1373,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1">
@@ -1381,7 +1381,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1493,7 +1493,7 @@
         <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1501,7 +1501,7 @@
         <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1509,7 +1509,7 @@
         <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1530,7 +1530,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
         <v>102</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1565,7 +1565,7 @@
         <v>54</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1573,7 +1573,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1581,15 +1581,15 @@
         <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
         <v>135</v>
-      </c>
-      <c r="B41" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1608,7 +1608,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>

</xml_diff>

<commit_message>
Replace NA with "", add regex test for valid lines in px file
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_BEXSTA_small.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_BEXSTA_small.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB298E7-0EB2-46CC-B479-454346DF6605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B17106-45A7-4336-BFE9-A327BFD53979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18900" yWindow="12450" windowWidth="17520" windowHeight="12195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17265" yWindow="0" windowWidth="23220" windowHeight="31800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="140">
   <si>
     <t>VarName</t>
   </si>
@@ -374,9 +374,6 @@
   </si>
   <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>Befolkningsstatistikregistret indeholder …</t>
   </si>
   <si>
     <t>CHARSET</t>
@@ -843,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -966,13 +963,13 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J3" t="s">
         <v>83</v>
@@ -984,18 +981,18 @@
         <v>84</v>
       </c>
       <c r="M3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" t="s">
         <v>136</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>137</v>
-      </c>
-      <c r="O3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
         <v>73</v>
@@ -1254,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1274,15 +1271,15 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="4">
         <v>2000</v>
@@ -1290,26 +1287,26 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1338,51 +1335,45 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1">
       <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1">
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
@@ -1530,7 +1521,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
         <v>102</v>
@@ -1546,7 +1537,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1554,7 +1545,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1586,10 +1577,10 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" t="s">
         <v>134</v>
-      </c>
-      <c r="B41" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>